<commit_message>
Updated parts list to as-biult
</commit_message>
<xml_diff>
--- a/Hardware design/Open Door Parts List.xlsx
+++ b/Hardware design/Open Door Parts List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="63">
   <si>
     <t>Item #</t>
   </si>
@@ -48,9 +48,6 @@
     <t>https://store.particle.io/collections/photon</t>
   </si>
   <si>
-    <t>Particle Photon WiFi Module with headers</t>
-  </si>
-  <si>
     <t>Relay Shield</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>Electric door strike, NC/fail secure, 12 VDC, suitable for wood door frame.</t>
   </si>
   <si>
-    <t>Diode, general purpose, 1A</t>
-  </si>
-  <si>
     <t>Many alternatives are available in all prices/quality.</t>
   </si>
   <si>
@@ -84,45 +78,15 @@
     <t>Optional: For housing the relay shield/photon</t>
   </si>
   <si>
-    <t>Resistor, 1 Kohm, 1/4 watt</t>
-  </si>
-  <si>
-    <t>LED, 5 mm, Green</t>
-  </si>
-  <si>
     <t>Generic Electric Strike Fail Secure</t>
   </si>
   <si>
-    <t>http://www.jameco.com/z/CF1-4W102JRC-Resistor-Carbon-Film-1k-Ohm-1-4-Watt-5-In-Bags-of-10-and-100-_690865.html</t>
-  </si>
-  <si>
-    <t>Optional: for indicator LED; ; bag of 10 resistors</t>
-  </si>
-  <si>
-    <t>http://www.jameco.com/z/LG3330-LED-Uni-Color-Green-565nm-2-Pin-T-1-3-4_34761.html</t>
-  </si>
-  <si>
-    <t>Optional: for indicator LED; bag of 10</t>
-  </si>
-  <si>
-    <t>http://www.jameco.com/z/1N4004-Major-Brands-400-VOLT-1-AMP-DO-41-SILICON-RECTIFIER-DIODE_35991.html</t>
-  </si>
-  <si>
-    <t>1N4004</t>
-  </si>
-  <si>
     <t>Flyback diode to protect relay contacts from inductive loads; bag of 10</t>
   </si>
   <si>
     <t>http://www.officedepot.com/a/products/452396/Really-Useful-Boxes-Plastic-Storage-Box/</t>
   </si>
   <si>
-    <t>2 wire insulated doorbell or sprinkler cable. 18 AWG solid wire.</t>
-  </si>
-  <si>
-    <t>for connecting strike plate to relay module.  Length depends upon installation.  Purchase as needed at Home Depot</t>
-  </si>
-  <si>
     <t>Total:</t>
   </si>
   <si>
@@ -138,13 +102,109 @@
     <t>Jameco</t>
   </si>
   <si>
-    <t>Office Depot</t>
-  </si>
-  <si>
-    <t>Home Depot</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/Generic-Electric-Strike-Secure-Control/dp/B00V45GWTI/ref=sr_1_1?s=hi&amp;ie=UTF8&amp;qid=1469666361&amp;sr=1-1&amp;keywords=generic+electric+strike</t>
+  </si>
+  <si>
+    <t>Jameco #231010</t>
+  </si>
+  <si>
+    <t>Jameco #659382</t>
+  </si>
+  <si>
+    <t>Terminal block, 6 column x 2 row; 140 series</t>
+  </si>
+  <si>
+    <t>Terminal block shorting jumper for 140 series, 140J-1</t>
+  </si>
+  <si>
+    <t>OfficeMax #452396</t>
+  </si>
+  <si>
+    <t>http://www.jameco.com/webapp/wcs/stores/servlet/ProductDisplay?search_type=jamecoall&amp;catalogId=10001&amp;freeText=231010&amp;langId=-1&amp;productId=231010&amp;storeId=10001&amp;ddkey=http:StoreCatalogDrillDownView</t>
+  </si>
+  <si>
+    <t>http://www.jameco.com/webapp/wcs/stores/servlet/ProductDisplay?search_type=jamecoall&amp;catalogId=10001&amp;freeText=659382&amp;langId=-1&amp;productId=659382&amp;storeId=10001&amp;ddkey=http:StoreCatalogDrillDownView</t>
+  </si>
+  <si>
+    <t>Resistor, 680 ohm, 1/2 watt</t>
+  </si>
+  <si>
+    <t>Frys #999156</t>
+  </si>
+  <si>
+    <t>Frys Electronics</t>
+  </si>
+  <si>
+    <t>http://www.frys.com/search?search_type=regular&amp;sqxts=1&amp;cat=&amp;query_string=HW168</t>
+  </si>
+  <si>
+    <t>http://www.frys.com/product/1334056?site=sr:SEARCH:MAIN_RSLT_PG</t>
+  </si>
+  <si>
+    <t>Frys #334056</t>
+  </si>
+  <si>
+    <t>Green LED panel mount indicator; 20 ms, no internal resistor</t>
+  </si>
+  <si>
+    <t>Optional: current limit resistor for indicator LED</t>
+  </si>
+  <si>
+    <t>Optional: LED indicator, panel mount, no internal current limit resistor.</t>
+  </si>
+  <si>
+    <t>Frys #1975293</t>
+  </si>
+  <si>
+    <t>Diode, general purpose, 1A, NTE 587 or equivalent</t>
+  </si>
+  <si>
+    <t>http://www.frys.com/product/1975293?site=sr:SEARCH:MAIN_RSLT_PG</t>
+  </si>
+  <si>
+    <t>Office Depot/Office Max</t>
+  </si>
+  <si>
+    <t>Hookup wire, #22 AWG or thicker</t>
+  </si>
+  <si>
+    <t>Misc</t>
+  </si>
+  <si>
+    <t>Hookup wire as needed for installation</t>
+  </si>
+  <si>
+    <t>Nylon standoff, 1/2", female-female, #4-40 threaded</t>
+  </si>
+  <si>
+    <t>Nylon screw, 1/4" long, #4-40 thread</t>
+  </si>
+  <si>
+    <t>Optional: for mounting Relay Board in pencil box</t>
+  </si>
+  <si>
+    <t>Wood screws, wall anchors, etc. for installation</t>
+  </si>
+  <si>
+    <t>Hardware as needed to mount terminal boack, pencil box, and door strike in the facility</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Keystone-Electronics/1902C/?qs=sGAEpiMZZMtrde5aJd3qw3QaZpWtG6nidQne%2f0XWhd0%3d</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>Mouser #534-1902C</t>
+  </si>
+  <si>
+    <t>Mouser #534-9527</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Keystone-Electronics/9527/?qs=sGAEpiMZZMtFmYSM%2fWUJwjMM2jkmYE8T6M5YAr%2f3kG0%3d</t>
+  </si>
+  <si>
+    <t>Particle Photon WiFi Module, with headers</t>
   </si>
 </sst>
 </file>
@@ -527,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -553,7 +613,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>2</v>
@@ -582,10 +642,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -607,13 +667,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -622,26 +682,26 @@
         <v>30</v>
       </c>
       <c r="G3" s="4">
-        <f t="shared" ref="G3:G10" si="0">F3*E3</f>
+        <f t="shared" ref="G3:G13" si="0">F3*E3</f>
         <v>30</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="32.25" customHeight="1">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A10" si="1">A3+1</f>
+        <f t="shared" ref="A4:A15" si="1">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
@@ -654,7 +714,7 @@
         <v>4.6900000000000004</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="31.5" customHeight="1">
@@ -663,13 +723,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2">
         <v>1</v>
@@ -682,174 +742,310 @@
         <v>23.6</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="30">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="45">
       <c r="A6" s="2">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
       </c>
       <c r="F6" s="4">
-        <v>0.5</v>
+        <v>1.29</v>
       </c>
       <c r="G6" s="4">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1.29</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="44.25" customHeight="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="78" customHeight="1">
       <c r="A7" s="2">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
+      <c r="B7" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="C7" s="5" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E7" s="2">
         <v>1</v>
       </c>
       <c r="F7" s="4">
-        <v>2</v>
+        <v>2.75</v>
       </c>
       <c r="G7" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I7" s="5" t="s">
+        <v>2.75</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30">
+    <row r="8" spans="1:9" ht="79.5" customHeight="1">
       <c r="A8" s="2">
-        <f t="shared" si="1"/>
+        <f>A7+1</f>
         <v>7</v>
       </c>
+      <c r="B8" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="C8" s="5" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E8" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F8" s="4">
-        <v>2.99</v>
+        <v>0.39</v>
       </c>
       <c r="G8" s="4">
         <f t="shared" si="0"/>
-        <v>2.99</v>
+        <v>1.17</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="34.5" customHeight="1">
       <c r="A9" s="2">
-        <f t="shared" si="1"/>
+        <f>A8+1</f>
         <v>8</v>
       </c>
+      <c r="B9" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="C9" s="5" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E9" s="2">
         <v>1</v>
       </c>
       <c r="F9" s="4">
-        <v>0.99</v>
+        <v>2.99</v>
       </c>
       <c r="G9" s="4">
         <f t="shared" si="0"/>
-        <v>0.99</v>
+        <v>2.99</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30">
       <c r="A10" s="2">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
+      <c r="B10" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="C10" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="E10" s="2">
         <v>1</v>
       </c>
       <c r="F10" s="4">
-        <v>1.5</v>
+        <v>1.49</v>
       </c>
       <c r="G10" s="4">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>1.49</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="9">
-        <f>SUM(G2:G11)</f>
-        <v>85.269999999999982</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="45" customHeight="1">
+      <c r="A11" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4">
+        <v>3.49</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="0"/>
+        <v>3.49</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="45" customHeight="1">
+      <c r="A12" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="2">
+        <v>4</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="0"/>
+        <v>3.2</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="52.5" customHeight="1">
+      <c r="A13" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="2">
+        <v>8</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="0"/>
+        <v>1.04</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="45" customHeight="1">
+      <c r="A14" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="45" customHeight="1">
+      <c r="A15" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="9">
+        <f>SUM(G2:G16)</f>
+        <v>94.71</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H3" r:id="rId1"/>
-    <hyperlink ref="H8" r:id="rId2"/>
+    <hyperlink ref="H9" r:id="rId2"/>
     <hyperlink ref="H5" r:id="rId3"/>
     <hyperlink ref="H4" r:id="rId4"/>
     <hyperlink ref="H2" r:id="rId5"/>
     <hyperlink ref="H6" r:id="rId6"/>
-    <hyperlink ref="H9" r:id="rId7"/>
-    <hyperlink ref="H10" r:id="rId8"/>
+    <hyperlink ref="H10" r:id="rId7"/>
+    <hyperlink ref="H7" r:id="rId8"/>
+    <hyperlink ref="H8" r:id="rId9"/>
+    <hyperlink ref="H11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>